<commit_message>
Berhasil Import Data Prakikan .XLSX
</commit_message>
<xml_diff>
--- a/_file/__format_data_praktikan.xlsx
+++ b/_file/__format_data_praktikan.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>NO.</t>
   </si>
@@ -56,118 +56,10 @@
     <t>NIM / NPM / NIS</t>
   </si>
   <si>
-    <t>ADE IHSAN MR.</t>
+    <t>PROGRAM STUDI</t>
   </si>
   <si>
-    <t>RANI RIFFANI</t>
-  </si>
-  <si>
-    <t>FAJAR RACHMAT HERMANSYAH</t>
-  </si>
-  <si>
-    <t>SITHA RAMADHANI A.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RIZKI EGI </t>
-  </si>
-  <si>
-    <t>LUKMAN SALEHUDIN</t>
-  </si>
-  <si>
-    <t>ASEP SAEPUDIN</t>
-  </si>
-  <si>
-    <t>FERLISTIAN RIZKI</t>
-  </si>
-  <si>
-    <t>ARIF HAKIM</t>
-  </si>
-  <si>
-    <t>ADI HARDIANSYAH</t>
-  </si>
-  <si>
-    <t>NANDANG</t>
-  </si>
-  <si>
-    <t>0891278318723</t>
-  </si>
-  <si>
-    <t>087623918732</t>
-  </si>
-  <si>
-    <t>0822891238911</t>
-  </si>
-  <si>
-    <t>0889263223683</t>
-  </si>
-  <si>
-    <t>0898298332323</t>
-  </si>
-  <si>
-    <t>0822237891722</t>
-  </si>
-  <si>
-    <t>0822337031729</t>
-  </si>
-  <si>
-    <t>0822113232311</t>
-  </si>
-  <si>
-    <t>0822237001728</t>
-  </si>
-  <si>
-    <t>0811209312322</t>
-  </si>
-  <si>
-    <t>0812312329822</t>
-  </si>
-  <si>
-    <t>0892831238723</t>
-  </si>
-  <si>
-    <t>adeamr@gmail.com</t>
-  </si>
-  <si>
-    <t>asep@gmail.com</t>
-  </si>
-  <si>
-    <t>fajar@gmail.com</t>
-  </si>
-  <si>
-    <t>ferlis@gmail.com</t>
-  </si>
-  <si>
-    <t>lukman@gmail.com</t>
-  </si>
-  <si>
-    <t>raniriff@gmail.com</t>
-  </si>
-  <si>
-    <t>egi.rizki@gmail.com</t>
-  </si>
-  <si>
-    <t>ramasd123@gmail.com</t>
-  </si>
-  <si>
-    <t>arif_hakim@gmail.com</t>
-  </si>
-  <si>
-    <t>adihhardianr@gmail.com</t>
-  </si>
-  <si>
-    <t>nandang@gmail.com</t>
-  </si>
-  <si>
-    <t>KOTA BANDUNG</t>
-  </si>
-  <si>
-    <t>KAB. BANDUNG</t>
-  </si>
-  <si>
-    <t>KOTA CIMAHI</t>
-  </si>
-  <si>
-    <t>KAB. BANDUNG BARAT</t>
+    <t>INSTITUSI</t>
   </si>
 </sst>
 </file>
@@ -288,10 +180,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -323,7 +214,6 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -341,6 +231,15 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -657,22 +556,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="33" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="258" width="9.140625" style="1"/>
+    <col min="2" max="2" width="30.140625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="33" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="33" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="258" width="9.140625" style="1"/>
     <col min="259" max="259" width="16.42578125" style="1" customWidth="1"/>
     <col min="260" max="260" width="39.7109375" style="1" customWidth="1"/>
     <col min="261" max="261" width="17.5703125" style="1" customWidth="1"/>
@@ -1053,380 +952,294 @@
     <col min="16136" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:9" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+      <c r="H1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="C2" s="6">
-        <v>1010202201</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="C3" s="6">
-        <v>1010202202</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="6">
-        <v>1010202203</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="C5" s="6">
-        <v>1010202204</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="6">
-        <v>1010202205</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>3</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="6">
-        <v>1010202206</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="6">
-        <v>1010202207</v>
-      </c>
-      <c r="D8" s="16" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="6">
-        <v>1010202208</v>
-      </c>
-      <c r="D9" s="16" t="s">
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="6">
-        <v>1010202209</v>
-      </c>
-      <c r="D10" s="17" t="s">
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="6">
-        <v>1010202210</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="6">
-        <v>1010202211</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
-        <v>16</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
-        <v>18</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
-        <v>19</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
-        <v>20</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1">
@@ -1434,21 +1247,7 @@
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3:F12" r:id="rId2" display="adeamr@gmail.com"/>
-    <hyperlink ref="F3" r:id="rId3"/>
-    <hyperlink ref="F4" r:id="rId4"/>
-    <hyperlink ref="F5" r:id="rId5"/>
-    <hyperlink ref="F6" r:id="rId6"/>
-    <hyperlink ref="F7" r:id="rId7"/>
-    <hyperlink ref="F8" r:id="rId8"/>
-    <hyperlink ref="F9" r:id="rId9"/>
-    <hyperlink ref="F10" r:id="rId10"/>
-    <hyperlink ref="F11" r:id="rId11"/>
-    <hyperlink ref="F12" r:id="rId12"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId13"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>